<commit_message>
Implemented Trash features with soft delete of files[ADD]
</commit_message>
<xml_diff>
--- a/Detailed_API_Documentation-2.xlsx
+++ b/Detailed_API_Documentation-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/presidio/Downloads/Group-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69660410-4D8C-0943-83CB-75D005CCB27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2715EACB-AA91-C945-B824-95DE77F033B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="500" windowWidth="26200" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="116">
   <si>
     <t>Controller</t>
   </si>
@@ -400,6 +400,59 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Bulk Download File</t>
+  </si>
+  <si>
+    <t>/api/v1/files/bulk-download</t>
+  </si>
+  <si>
+    <t>Downloads file as ZIP format</t>
+  </si>
+  <si>
+    <t>{
+  "fileIds": [
+    "3fa85f64-5717-4562-b3fc-2c963f66afa6"
+  ],
+  "zipFileName": "string"
+}</t>
+  </si>
+  <si>
+    <t>Get all files in trash</t>
+  </si>
+  <si>
+    <t>/api/v1/files/trash</t>
+  </si>
+  <si>
+    <t>Returns list of files details in the trash</t>
+  </si>
+  <si>
+    <t>Restore from trash</t>
+  </si>
+  <si>
+    <t>Delete permanently in trash</t>
+  </si>
+  <si>
+    <t>Get trash stats</t>
+  </si>
+  <si>
+    <t>/api/v1/files/trash/stats</t>
+  </si>
+  <si>
+    <t>/api/v1/files/trash/{id}/permanent</t>
+  </si>
+  <si>
+    <t>/api/v1/files/trash/{id}/restore</t>
+  </si>
+  <si>
+    <t>Move file form trash to Archive file &amp; make db update</t>
+  </si>
+  <si>
+    <t>Removes file at the trash &amp; also in archieve if exist</t>
+  </si>
+  <si>
+    <t>Get trash statistics</t>
   </si>
 </sst>
 </file>
@@ -751,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -976,121 +1029,121 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>24</v>
@@ -1098,77 +1151,71 @@
       <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>24</v>
@@ -1176,137 +1223,265 @@
       <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>